<commit_message>
Updates for this term.
</commit_message>
<xml_diff>
--- a/Labs/Lab01/Lab01Rubric_CS195.xlsx
+++ b/Labs/Lab01/Lab01Rubric_CS195.xlsx
@@ -1,43 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\CIS195-CourseMaterials\LabStarters\Lab01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CIS195-CourseMaterials/Labs/Lab01/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A4334F9-C307-4D1E-8EC2-744226AF76D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864E7E81-B7EB-0840-9D07-0E2F5CEFA3A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5748" yWindow="1284" windowWidth="22944" windowHeight="11592" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
+    <workbookView xWindow="5740" yWindow="2620" windowWidth="18860" windowHeight="13060" activeTab="1" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
     <sheet name="Grade" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>Requirements:</t>
   </si>
@@ -88,6 +77,9 @@
   </si>
   <si>
     <t>ol and ul (one of each)</t>
+  </si>
+  <si>
+    <t>Comments</t>
   </si>
 </sst>
 </file>
@@ -168,7 +160,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,22 +482,22 @@
   </sheetPr>
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection sqref="A1:C14"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.19921875" customWidth="1"/>
+    <col min="1" max="1" width="24.1640625" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -512,7 +506,7 @@
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -520,7 +514,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -528,7 +522,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -536,7 +530,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -544,7 +538,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -552,7 +546,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -560,7 +554,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -568,7 +562,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -576,16 +570,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>9</v>
       </c>
@@ -595,27 +589,27 @@
       </c>
       <c r="C14" s="4"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -628,77 +622,97 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96879333-0874-3847-ABBB-D0DF183A7724}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.69921875" customWidth="1"/>
-    <col min="2" max="2" width="7.69921875" customWidth="1"/>
-    <col min="3" max="3" width="6.09765625" customWidth="1"/>
-    <col min="4" max="4" width="17.5" style="5" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" customWidth="1"/>
+    <col min="3" max="3" width="6.1640625" customWidth="1"/>
+    <col min="4" max="4" width="1" style="5" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
       <c r="D3" s="7"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="E3" s="7"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B7">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C7">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="E7" s="6"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -706,32 +720,35 @@
       <c r="C9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B11">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C11">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B12">
         <v>5</v>
@@ -739,75 +756,71 @@
       <c r="C12">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B13">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C13">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14">
-        <v>3</v>
-      </c>
-      <c r="C14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="4">
-        <f>SUM(B7:B14)</f>
+      <c r="B16" s="4">
+        <f>SUM(B6:B13)</f>
         <v>40</v>
       </c>
-      <c r="C17" s="4">
-        <f>SUM(C7:C14)</f>
+      <c r="C16" s="4">
+        <f>SUM(C6:C13)</f>
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="3"/>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A3:D3"/>
+  <mergeCells count="2">
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>